<commit_message>
update test cases files
</commit_message>
<xml_diff>
--- a/testCases/testCases.xlsx
+++ b/testCases/testCases.xlsx
@@ -1,49 +1,131 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlinelavigne/PycharmProjects/ebayProject/testCases/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048A37E6-BBAA-8D45-BEF2-E2D04A217405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Home Page" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Home Page" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+  <si>
+    <t>Test case ID</t>
+  </si>
+  <si>
+    <t>Test Case Title</t>
+  </si>
+  <si>
+    <t>Pre-requisites</t>
+  </si>
+  <si>
+    <t>Steps To Reproduce</t>
+  </si>
+  <si>
+    <t>Test Data</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>TC_HP_001</t>
+  </si>
+  <si>
+    <t>Home Page is loaded after user reaches the Home Page</t>
+  </si>
+  <si>
+    <t>Open the URL (https://www.ebay.ca/) of the application in any browser</t>
+  </si>
+  <si>
+    <t>All elements of the Home Page are visible (e.g. navbar, search field, personalized selection of products etc.)</t>
+  </si>
+  <si>
+    <t>P0</t>
+  </si>
+  <si>
+    <t>TC_HP_002</t>
+  </si>
+  <si>
+    <t>User can search a product in the search box by category</t>
+  </si>
+  <si>
+    <t>1. Enter [Search_input] in the search box
+2. Select [Search_category] in the category field
+3. Click the 'Search' button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Search_input]
+DataEbay.xlsx col A*
+[Search_category]
+dataEbay.xlsx col B*
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiple results matching the searched products and the category selected are displayed </t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>PENDING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*Please see DataEbay.xlsx in TestData </t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="14"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <i val="1"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -62,14 +144,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFFFFF"/>
-        <bgColor rgb="00FFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00C9F297"/>
-        <bgColor rgb="00C9F297"/>
+        <fgColor theme="0"/>
+        <bgColor rgb="FFC9F297"/>
       </patternFill>
     </fill>
   </fills>
@@ -214,130 +290,65 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="16">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -637,11 +648,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
@@ -649,160 +656,106 @@
       <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col width="13.5" customWidth="1" min="1" max="1"/>
-    <col width="58.1640625" customWidth="1" min="2" max="2"/>
-    <col width="39.6640625" customWidth="1" min="3" max="3"/>
-    <col width="39" customWidth="1" min="4" max="4"/>
-    <col width="25.5" customWidth="1" min="5" max="5"/>
-    <col width="28" customWidth="1" min="6" max="6"/>
-    <col width="18.5" customWidth="1" min="7" max="7"/>
-    <col width="17.6640625" customWidth="1" min="8" max="8"/>
-    <col width="20.5" customWidth="1" min="9" max="9"/>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="58.1640625" customWidth="1"/>
+    <col min="3" max="3" width="39.6640625" customWidth="1"/>
+    <col min="4" max="4" width="39" customWidth="1"/>
+    <col min="5" max="5" width="25.5" customWidth="1"/>
+    <col min="6" max="6" width="28" customWidth="1"/>
+    <col min="7" max="7" width="18.5" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" customWidth="1"/>
+    <col min="9" max="9" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="21" customHeight="1" thickBot="1">
-      <c r="A1" s="8" t="inlineStr">
-        <is>
-          <t>Test case ID</t>
-        </is>
-      </c>
-      <c r="B1" s="9" t="inlineStr">
-        <is>
-          <t>Test Case Title</t>
-        </is>
-      </c>
-      <c r="C1" s="9" t="inlineStr">
-        <is>
-          <t>Pre-requisites</t>
-        </is>
-      </c>
-      <c r="D1" s="9" t="inlineStr">
-        <is>
-          <t>Steps To Reproduce</t>
-        </is>
-      </c>
-      <c r="E1" s="9" t="inlineStr">
-        <is>
-          <t>Test Data</t>
-        </is>
-      </c>
-      <c r="F1" s="9" t="inlineStr">
-        <is>
-          <t>Expected Result</t>
-        </is>
-      </c>
-      <c r="G1" s="9" t="inlineStr">
-        <is>
-          <t>Priority</t>
-        </is>
-      </c>
-      <c r="H1" s="9" t="inlineStr">
-        <is>
-          <t>Result</t>
-        </is>
-      </c>
-      <c r="I1" s="10" t="inlineStr">
-        <is>
-          <t>Notes</t>
-        </is>
+    <row r="1" spans="1:9" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="2" ht="68" customHeight="1">
-      <c r="A2" s="5" t="inlineStr">
-        <is>
-          <t>TC_HP_001</t>
-        </is>
-      </c>
-      <c r="B2" s="6" t="inlineStr">
-        <is>
-          <t>Home Page is loaded after user reaches the Home Page</t>
-        </is>
-      </c>
-      <c r="C2" s="6" t="inlineStr">
-        <is>
-          <t>Open the URL (https://www.ebay.ca/) of the application in any browser</t>
-        </is>
-      </c>
-      <c r="D2" s="6" t="n"/>
-      <c r="E2" s="11" t="n"/>
-      <c r="F2" s="6" t="inlineStr">
-        <is>
-          <t>All elements of the Home Page are visible (e.g. navbar, search field, personalized selection of products etc.)</t>
-        </is>
-      </c>
-      <c r="G2" s="7" t="inlineStr">
-        <is>
-          <t>P0</t>
-        </is>
-      </c>
-      <c r="H2" s="17" t="inlineStr">
-        <is>
-          <t>PASS</t>
-        </is>
-      </c>
-      <c r="I2" s="15" t="n"/>
+    <row r="2" spans="1:9" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="14"/>
     </row>
-    <row r="3" ht="103" customHeight="1" thickBot="1">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>TC_HP_002</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>User can search a product in the search box by category</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>Open the URL (https://www.ebay.ca/) of the application in any browser</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>1. Enter [Search_input] in the search box
-2. Select [Search_category] in the category field
-3. Click the 'Search' button</t>
-        </is>
-      </c>
-      <c r="E3" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">[Search_input]
-DataEbay.xlsx col A*
-[Search_category]
-dataEbay.xlsx col B*
-</t>
-        </is>
-      </c>
-      <c r="F3" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Multiple results matching the searched products and the category selected are displayed </t>
-        </is>
-      </c>
-      <c r="G3" s="4" t="inlineStr">
-        <is>
-          <t>P1</t>
-        </is>
-      </c>
-      <c r="H3" s="14" t="inlineStr">
-        <is>
-          <t>PENDING</t>
-        </is>
-      </c>
-      <c r="I3" s="3" t="n"/>
+    <row r="3" spans="1:9" ht="103" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="3"/>
     </row>
-    <row r="6">
-      <c r="A6" s="12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">*Please see DataEbay.xlsx in TestData </t>
-        </is>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="H2:H3" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H2:H3" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"PENDING, PASS, FAIL, CANNOT CHECK, N/A"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>